<commit_message>
fix bug pada export excel
</commit_message>
<xml_diff>
--- a/template/template_hse_report.xlsx
+++ b/template/template_hse_report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\HSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hse\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E2BF66-AF11-4EC2-9D7C-339D269BF4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A54E4E-77CE-4BC7-B601-870849157562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Great Wall Drilling Company
 Daily HSE Report</t>
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t>Observed personnel about to carry out lifting operation, however they still wearing light duty gloves. Stopped them and asked to change their gloves with impact gloves. They comply.</t>
-  </si>
-  <si>
-    <t>HSE &amp; Doctor - Sindu/Adi &amp; dr. Nurtanio</t>
   </si>
 </sst>
 </file>
@@ -1671,6 +1668,126 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1715,126 +1832,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="256">
@@ -2427,8 +2424,8 @@
   </sheetPr>
   <dimension ref="A1:AI3605"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A68" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="U82" sqref="U82"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7265625" defaultRowHeight="15.5"/>
@@ -2463,42 +2460,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="31.15" customHeight="1">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="56"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="95"/>
+      <c r="P1" s="96"/>
     </row>
     <row r="2" spans="1:28">
-      <c r="A2" s="57"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="59"/>
+      <c r="A2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="99"/>
     </row>
     <row r="3" spans="1:28">
       <c r="A3" s="5" t="s">
@@ -2569,11 +2566,11 @@
       <c r="P5" s="40"/>
     </row>
     <row r="6" spans="1:28">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="62"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="102"/>
       <c r="D6" s="15"/>
       <c r="E6" s="14" t="s">
         <v>8</v>
@@ -2583,50 +2580,50 @@
         <v>9</v>
       </c>
       <c r="H6" s="17"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64"/>
-      <c r="N6" s="64"/>
-      <c r="O6" s="64"/>
-      <c r="P6" s="65"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="104"/>
+      <c r="K6" s="104"/>
+      <c r="L6" s="104"/>
+      <c r="M6" s="104"/>
+      <c r="N6" s="104"/>
+      <c r="O6" s="104"/>
+      <c r="P6" s="105"/>
     </row>
     <row r="7" spans="1:28" ht="18.649999999999999" customHeight="1">
-      <c r="A7" s="66"/>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="67"/>
-      <c r="N7" s="67"/>
-      <c r="O7" s="67"/>
-      <c r="P7" s="68"/>
+      <c r="A7" s="106"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="107"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="107"/>
+      <c r="N7" s="107"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="108"/>
     </row>
     <row r="8" spans="1:28" ht="78" customHeight="1">
-      <c r="A8" s="69"/>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="70"/>
-      <c r="N8" s="70"/>
-      <c r="O8" s="70"/>
-      <c r="P8" s="71"/>
+      <c r="A8" s="89"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
+      <c r="N8" s="90"/>
+      <c r="O8" s="90"/>
+      <c r="P8" s="91"/>
       <c r="AB8" s="3" t="s">
         <v>10</v>
       </c>
@@ -2638,22 +2635,22 @@
       <c r="B9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
-      <c r="N9" s="72"/>
-      <c r="O9" s="72"/>
-      <c r="P9" s="73"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="92"/>
+      <c r="L9" s="92"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="92"/>
+      <c r="O9" s="92"/>
+      <c r="P9" s="93"/>
       <c r="Q9" s="4" t="s">
         <v>14</v>
       </c>
@@ -2663,20 +2660,20 @@
         <v>1</v>
       </c>
       <c r="B10" s="21"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="75"/>
-      <c r="P10" s="76"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="87"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="87"/>
+      <c r="G10" s="87"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="87"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="87"/>
+      <c r="M10" s="87"/>
+      <c r="N10" s="87"/>
+      <c r="O10" s="87"/>
+      <c r="P10" s="88"/>
       <c r="Q10" s="46" t="s">
         <v>15</v>
       </c>
@@ -2687,20 +2684,20 @@
         <v>2</v>
       </c>
       <c r="B11" s="21"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="75"/>
-      <c r="P11" s="76"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="87"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="87"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="87"/>
+      <c r="P11" s="88"/>
       <c r="Q11" s="47"/>
     </row>
     <row r="12" spans="1:28" s="2" customFormat="1" ht="60" customHeight="1">
@@ -2708,20 +2705,20 @@
         <v>3</v>
       </c>
       <c r="B12" s="21"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="75"/>
-      <c r="L12" s="75"/>
-      <c r="M12" s="75"/>
-      <c r="N12" s="75"/>
-      <c r="O12" s="75"/>
-      <c r="P12" s="76"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="87"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="88"/>
       <c r="Q12" s="47"/>
     </row>
     <row r="13" spans="1:28" s="2" customFormat="1" ht="60" customHeight="1">
@@ -2729,20 +2726,20 @@
         <v>4</v>
       </c>
       <c r="B13" s="21"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="78"/>
-      <c r="M13" s="78"/>
-      <c r="N13" s="78"/>
-      <c r="O13" s="78"/>
-      <c r="P13" s="79"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="81"/>
+      <c r="N13" s="81"/>
+      <c r="O13" s="81"/>
+      <c r="P13" s="82"/>
       <c r="Q13" s="47"/>
     </row>
     <row r="14" spans="1:28" s="2" customFormat="1" ht="60" customHeight="1">
@@ -2750,20 +2747,20 @@
         <v>5</v>
       </c>
       <c r="B14" s="21"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78"/>
-      <c r="M14" s="78"/>
-      <c r="N14" s="78"/>
-      <c r="O14" s="78"/>
-      <c r="P14" s="79"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="81"/>
+      <c r="N14" s="81"/>
+      <c r="O14" s="81"/>
+      <c r="P14" s="82"/>
       <c r="Q14" s="47"/>
     </row>
     <row r="15" spans="1:28" s="2" customFormat="1" ht="60" customHeight="1">
@@ -2771,20 +2768,20 @@
         <v>6</v>
       </c>
       <c r="B15" s="21"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="75"/>
-      <c r="K15" s="75"/>
-      <c r="L15" s="75"/>
-      <c r="M15" s="75"/>
-      <c r="N15" s="75"/>
-      <c r="O15" s="75"/>
-      <c r="P15" s="76"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="87"/>
+      <c r="L15" s="87"/>
+      <c r="M15" s="87"/>
+      <c r="N15" s="87"/>
+      <c r="O15" s="87"/>
+      <c r="P15" s="88"/>
       <c r="Q15" s="47"/>
     </row>
     <row r="16" spans="1:28" s="2" customFormat="1" ht="60" customHeight="1">
@@ -2792,20 +2789,20 @@
         <v>7</v>
       </c>
       <c r="B16" s="21"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="75"/>
-      <c r="L16" s="75"/>
-      <c r="M16" s="75"/>
-      <c r="N16" s="75"/>
-      <c r="O16" s="75"/>
-      <c r="P16" s="76"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="87"/>
+      <c r="N16" s="87"/>
+      <c r="O16" s="87"/>
+      <c r="P16" s="88"/>
       <c r="Q16" s="47"/>
     </row>
     <row r="17" spans="1:35" s="2" customFormat="1" ht="60" customHeight="1">
@@ -2813,20 +2810,20 @@
         <v>8</v>
       </c>
       <c r="B17" s="21"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="75"/>
-      <c r="L17" s="75"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="75"/>
-      <c r="O17" s="75"/>
-      <c r="P17" s="76"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="87"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="87"/>
+      <c r="M17" s="87"/>
+      <c r="N17" s="87"/>
+      <c r="O17" s="87"/>
+      <c r="P17" s="88"/>
       <c r="Q17" s="47"/>
     </row>
     <row r="18" spans="1:35" s="2" customFormat="1" ht="60" customHeight="1">
@@ -2834,20 +2831,20 @@
         <v>9</v>
       </c>
       <c r="B18" s="21"/>
-      <c r="C18" s="77"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="78"/>
-      <c r="J18" s="78"/>
-      <c r="K18" s="78"/>
-      <c r="L18" s="78"/>
-      <c r="M18" s="78"/>
-      <c r="N18" s="78"/>
-      <c r="O18" s="78"/>
-      <c r="P18" s="79"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="81"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="81"/>
+      <c r="N18" s="81"/>
+      <c r="O18" s="81"/>
+      <c r="P18" s="82"/>
       <c r="Q18" s="47"/>
     </row>
     <row r="19" spans="1:35" s="2" customFormat="1" ht="60" customHeight="1">
@@ -2855,20 +2852,20 @@
         <v>10</v>
       </c>
       <c r="B19" s="21"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
-      <c r="K19" s="78"/>
-      <c r="L19" s="78"/>
-      <c r="M19" s="78"/>
-      <c r="N19" s="78"/>
-      <c r="O19" s="78"/>
-      <c r="P19" s="79"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="81"/>
+      <c r="N19" s="81"/>
+      <c r="O19" s="81"/>
+      <c r="P19" s="82"/>
       <c r="Q19" s="47"/>
     </row>
     <row r="20" spans="1:35" s="2" customFormat="1" ht="60" customHeight="1">
@@ -2876,20 +2873,20 @@
         <v>11</v>
       </c>
       <c r="B20" s="21"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="81"/>
-      <c r="G20" s="81"/>
-      <c r="H20" s="81"/>
-      <c r="I20" s="81"/>
-      <c r="J20" s="81"/>
-      <c r="K20" s="81"/>
-      <c r="L20" s="81"/>
-      <c r="M20" s="81"/>
-      <c r="N20" s="81"/>
-      <c r="O20" s="81"/>
-      <c r="P20" s="82"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="84"/>
+      <c r="G20" s="84"/>
+      <c r="H20" s="84"/>
+      <c r="I20" s="84"/>
+      <c r="J20" s="84"/>
+      <c r="K20" s="84"/>
+      <c r="L20" s="84"/>
+      <c r="M20" s="84"/>
+      <c r="N20" s="84"/>
+      <c r="O20" s="84"/>
+      <c r="P20" s="85"/>
       <c r="Q20" s="47"/>
     </row>
     <row r="21" spans="1:35" s="2" customFormat="1" ht="60" customHeight="1">
@@ -2897,20 +2894,20 @@
         <v>12</v>
       </c>
       <c r="B21" s="21"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="75"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="75"/>
-      <c r="L21" s="75"/>
-      <c r="M21" s="75"/>
-      <c r="N21" s="75"/>
-      <c r="O21" s="75"/>
-      <c r="P21" s="76"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87"/>
+      <c r="H21" s="87"/>
+      <c r="I21" s="87"/>
+      <c r="J21" s="87"/>
+      <c r="K21" s="87"/>
+      <c r="L21" s="87"/>
+      <c r="M21" s="87"/>
+      <c r="N21" s="87"/>
+      <c r="O21" s="87"/>
+      <c r="P21" s="88"/>
       <c r="Q21" s="47"/>
     </row>
     <row r="22" spans="1:35" s="2" customFormat="1" ht="60" customHeight="1">
@@ -2918,20 +2915,20 @@
         <v>9</v>
       </c>
       <c r="B22" s="21"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="81"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="81"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="81"/>
-      <c r="O22" s="81"/>
-      <c r="P22" s="82"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="84"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="84"/>
+      <c r="K22" s="84"/>
+      <c r="L22" s="84"/>
+      <c r="M22" s="84"/>
+      <c r="N22" s="84"/>
+      <c r="O22" s="84"/>
+      <c r="P22" s="85"/>
       <c r="Q22" s="47" t="s">
         <v>16</v>
       </c>
@@ -2944,20 +2941,20 @@
         <v>10</v>
       </c>
       <c r="B23" s="22"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="84"/>
-      <c r="K23" s="84"/>
-      <c r="L23" s="84"/>
-      <c r="M23" s="84"/>
-      <c r="N23" s="84"/>
-      <c r="O23" s="84"/>
-      <c r="P23" s="85"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="71"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="71"/>
+      <c r="N23" s="71"/>
+      <c r="O23" s="71"/>
+      <c r="P23" s="72"/>
       <c r="Q23" s="47" t="s">
         <v>17</v>
       </c>
@@ -2968,20 +2965,20 @@
         <v>11</v>
       </c>
       <c r="B24" s="22"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="84"/>
-      <c r="G24" s="84"/>
-      <c r="H24" s="84"/>
-      <c r="I24" s="84"/>
-      <c r="J24" s="84"/>
-      <c r="K24" s="84"/>
-      <c r="L24" s="84"/>
-      <c r="M24" s="84"/>
-      <c r="N24" s="84"/>
-      <c r="O24" s="84"/>
-      <c r="P24" s="85"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="71"/>
+      <c r="M24" s="71"/>
+      <c r="N24" s="71"/>
+      <c r="O24" s="71"/>
+      <c r="P24" s="72"/>
       <c r="Q24" s="47" t="s">
         <v>18</v>
       </c>
@@ -2991,20 +2988,20 @@
         <v>12</v>
       </c>
       <c r="B25" s="22"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="84"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="84"/>
-      <c r="H25" s="84"/>
-      <c r="I25" s="84"/>
-      <c r="J25" s="84"/>
-      <c r="K25" s="84"/>
-      <c r="L25" s="84"/>
-      <c r="M25" s="84"/>
-      <c r="N25" s="84"/>
-      <c r="O25" s="84"/>
-      <c r="P25" s="85"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="71"/>
+      <c r="M25" s="71"/>
+      <c r="N25" s="71"/>
+      <c r="O25" s="71"/>
+      <c r="P25" s="72"/>
       <c r="Q25" s="47" t="s">
         <v>19</v>
       </c>
@@ -3014,20 +3011,20 @@
         <v>13</v>
       </c>
       <c r="B26" s="22"/>
-      <c r="C26" s="83"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="84"/>
-      <c r="F26" s="84"/>
-      <c r="G26" s="84"/>
-      <c r="H26" s="84"/>
-      <c r="I26" s="84"/>
-      <c r="J26" s="84"/>
-      <c r="K26" s="84"/>
-      <c r="L26" s="84"/>
-      <c r="M26" s="84"/>
-      <c r="N26" s="84"/>
-      <c r="O26" s="84"/>
-      <c r="P26" s="85"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="71"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="71"/>
+      <c r="M26" s="71"/>
+      <c r="N26" s="71"/>
+      <c r="O26" s="71"/>
+      <c r="P26" s="72"/>
       <c r="Q26" s="47" t="s">
         <v>20</v>
       </c>
@@ -3037,20 +3034,20 @@
         <v>14</v>
       </c>
       <c r="B27" s="22"/>
-      <c r="C27" s="83"/>
-      <c r="D27" s="84"/>
-      <c r="E27" s="84"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="84"/>
-      <c r="H27" s="84"/>
-      <c r="I27" s="84"/>
-      <c r="J27" s="84"/>
-      <c r="K27" s="84"/>
-      <c r="L27" s="84"/>
-      <c r="M27" s="84"/>
-      <c r="N27" s="84"/>
-      <c r="O27" s="84"/>
-      <c r="P27" s="85"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="71"/>
+      <c r="J27" s="71"/>
+      <c r="K27" s="71"/>
+      <c r="L27" s="71"/>
+      <c r="M27" s="71"/>
+      <c r="N27" s="71"/>
+      <c r="O27" s="71"/>
+      <c r="P27" s="72"/>
       <c r="Q27" s="47" t="s">
         <v>21</v>
       </c>
@@ -3060,20 +3057,20 @@
         <v>15</v>
       </c>
       <c r="B28" s="22"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="84"/>
-      <c r="I28" s="84"/>
-      <c r="J28" s="84"/>
-      <c r="K28" s="84"/>
-      <c r="L28" s="84"/>
-      <c r="M28" s="84"/>
-      <c r="N28" s="84"/>
-      <c r="O28" s="84"/>
-      <c r="P28" s="85"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="71"/>
+      <c r="M28" s="71"/>
+      <c r="N28" s="71"/>
+      <c r="O28" s="71"/>
+      <c r="P28" s="72"/>
       <c r="Q28" s="47" t="s">
         <v>22</v>
       </c>
@@ -3119,29 +3116,29 @@
     <row r="49" spans="1:16" ht="14.5" customHeight="1"/>
     <row r="50" spans="1:16" ht="14.5" customHeight="1"/>
     <row r="51" spans="1:16" ht="16" thickBot="1">
-      <c r="A51" s="86" t="s">
+      <c r="A51" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="B51" s="87"/>
-      <c r="C51" s="87"/>
-      <c r="D51" s="87"/>
-      <c r="E51" s="87"/>
+      <c r="B51" s="74"/>
+      <c r="C51" s="74"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
       <c r="F51" s="23"/>
       <c r="G51" s="24"/>
       <c r="H51" s="24"/>
       <c r="I51" s="41"/>
-      <c r="J51" s="99"/>
-      <c r="K51" s="100"/>
-      <c r="L51" s="100"/>
-      <c r="M51" s="100"/>
-      <c r="N51" s="100"/>
-      <c r="O51" s="100"/>
-      <c r="P51" s="101"/>
+      <c r="J51" s="65"/>
+      <c r="K51" s="66"/>
+      <c r="L51" s="66"/>
+      <c r="M51" s="66"/>
+      <c r="N51" s="66"/>
+      <c r="O51" s="66"/>
+      <c r="P51" s="67"/>
     </row>
     <row r="52" spans="1:16">
-      <c r="A52" s="88"/>
-      <c r="B52" s="89"/>
-      <c r="C52" s="90"/>
+      <c r="A52" s="75"/>
+      <c r="B52" s="76"/>
+      <c r="C52" s="77"/>
       <c r="D52" s="25" t="s">
         <v>24</v>
       </c>
@@ -3154,78 +3151,78 @@
       <c r="G52" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="H52" s="91" t="s">
+      <c r="H52" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="I52" s="92"/>
-      <c r="J52" s="100"/>
-      <c r="K52" s="100"/>
-      <c r="L52" s="100"/>
-      <c r="M52" s="100"/>
-      <c r="N52" s="100"/>
-      <c r="O52" s="100"/>
-      <c r="P52" s="101"/>
+      <c r="I52" s="79"/>
+      <c r="J52" s="66"/>
+      <c r="K52" s="66"/>
+      <c r="L52" s="66"/>
+      <c r="M52" s="66"/>
+      <c r="N52" s="66"/>
+      <c r="O52" s="66"/>
+      <c r="P52" s="67"/>
     </row>
     <row r="53" spans="1:16" ht="17.25" customHeight="1">
-      <c r="A53" s="93"/>
-      <c r="B53" s="94"/>
-      <c r="C53" s="94"/>
+      <c r="A53" s="59"/>
+      <c r="B53" s="60"/>
+      <c r="C53" s="60"/>
       <c r="D53" s="26"/>
       <c r="E53" s="26"/>
       <c r="F53" s="26"/>
       <c r="G53" s="26"/>
       <c r="H53" s="27"/>
       <c r="I53" s="42"/>
-      <c r="J53" s="100"/>
-      <c r="K53" s="100"/>
-      <c r="L53" s="100"/>
-      <c r="M53" s="100"/>
-      <c r="N53" s="100"/>
-      <c r="O53" s="100"/>
-      <c r="P53" s="101"/>
+      <c r="J53" s="66"/>
+      <c r="K53" s="66"/>
+      <c r="L53" s="66"/>
+      <c r="M53" s="66"/>
+      <c r="N53" s="66"/>
+      <c r="O53" s="66"/>
+      <c r="P53" s="67"/>
     </row>
     <row r="54" spans="1:16" ht="16" thickBot="1">
-      <c r="A54" s="93"/>
-      <c r="B54" s="94"/>
-      <c r="C54" s="94"/>
+      <c r="A54" s="59"/>
+      <c r="B54" s="60"/>
+      <c r="C54" s="60"/>
       <c r="D54" s="26"/>
       <c r="E54" s="26"/>
       <c r="F54" s="26"/>
       <c r="G54" s="26"/>
       <c r="H54" s="27"/>
       <c r="I54" s="42"/>
-      <c r="J54" s="102"/>
-      <c r="K54" s="102"/>
-      <c r="L54" s="102"/>
-      <c r="M54" s="102"/>
-      <c r="N54" s="102"/>
-      <c r="O54" s="102"/>
-      <c r="P54" s="103"/>
+      <c r="J54" s="68"/>
+      <c r="K54" s="68"/>
+      <c r="L54" s="68"/>
+      <c r="M54" s="68"/>
+      <c r="N54" s="68"/>
+      <c r="O54" s="68"/>
+      <c r="P54" s="69"/>
     </row>
     <row r="55" spans="1:16">
-      <c r="A55" s="93"/>
-      <c r="B55" s="94"/>
-      <c r="C55" s="94"/>
+      <c r="A55" s="59"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="60"/>
       <c r="D55" s="26"/>
       <c r="E55" s="26"/>
       <c r="F55" s="26"/>
       <c r="G55" s="26"/>
       <c r="H55" s="27"/>
       <c r="I55" s="42"/>
-      <c r="J55" s="95" t="s">
+      <c r="J55" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="K55" s="95"/>
-      <c r="L55" s="95"/>
-      <c r="M55" s="95"/>
-      <c r="N55" s="95"/>
-      <c r="O55" s="95"/>
-      <c r="P55" s="96"/>
+      <c r="K55" s="61"/>
+      <c r="L55" s="61"/>
+      <c r="M55" s="61"/>
+      <c r="N55" s="61"/>
+      <c r="O55" s="61"/>
+      <c r="P55" s="62"/>
     </row>
     <row r="56" spans="1:16" ht="16" thickBot="1">
-      <c r="A56" s="97"/>
-      <c r="B56" s="98"/>
-      <c r="C56" s="98"/>
+      <c r="A56" s="63"/>
+      <c r="B56" s="64"/>
+      <c r="C56" s="64"/>
       <c r="D56" s="28"/>
       <c r="E56" s="28"/>
       <c r="F56" s="28"/>
@@ -3357,24 +3354,22 @@
       <c r="P84" s="45"/>
     </row>
     <row r="85" spans="1:16" ht="16" thickBot="1">
-      <c r="A85" s="104" t="s">
-        <v>39</v>
-      </c>
-      <c r="B85" s="105"/>
-      <c r="C85" s="106"/>
-      <c r="D85" s="107"/>
-      <c r="E85" s="106"/>
-      <c r="F85" s="106"/>
-      <c r="G85" s="106"/>
-      <c r="H85" s="106"/>
-      <c r="I85" s="106"/>
-      <c r="J85" s="106"/>
-      <c r="K85" s="106"/>
-      <c r="L85" s="106"/>
-      <c r="M85" s="106"/>
-      <c r="N85" s="106"/>
-      <c r="O85" s="106"/>
-      <c r="P85" s="108"/>
+      <c r="A85" s="54"/>
+      <c r="B85" s="55"/>
+      <c r="C85" s="56"/>
+      <c r="D85" s="57"/>
+      <c r="E85" s="56"/>
+      <c r="F85" s="56"/>
+      <c r="G85" s="56"/>
+      <c r="H85" s="56"/>
+      <c r="I85" s="56"/>
+      <c r="J85" s="56"/>
+      <c r="K85" s="56"/>
+      <c r="L85" s="56"/>
+      <c r="M85" s="56"/>
+      <c r="N85" s="56"/>
+      <c r="O85" s="56"/>
+      <c r="P85" s="58"/>
     </row>
     <row r="154" spans="4:11">
       <c r="D154" s="3"/>
@@ -3451,41 +3446,41 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="I6:P6"/>
+    <mergeCell ref="A7:P7"/>
+    <mergeCell ref="A8:P8"/>
+    <mergeCell ref="C9:P9"/>
+    <mergeCell ref="C10:P10"/>
+    <mergeCell ref="C11:P11"/>
+    <mergeCell ref="C12:P12"/>
+    <mergeCell ref="C13:P13"/>
+    <mergeCell ref="C14:P14"/>
+    <mergeCell ref="C15:P15"/>
+    <mergeCell ref="C16:P16"/>
+    <mergeCell ref="C17:P17"/>
+    <mergeCell ref="C18:P18"/>
+    <mergeCell ref="C19:P19"/>
+    <mergeCell ref="C20:P20"/>
+    <mergeCell ref="C21:P21"/>
+    <mergeCell ref="C22:P22"/>
+    <mergeCell ref="C23:P23"/>
+    <mergeCell ref="C24:P24"/>
+    <mergeCell ref="C25:P25"/>
+    <mergeCell ref="C26:P26"/>
+    <mergeCell ref="C27:P27"/>
+    <mergeCell ref="C28:P28"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="A53:C53"/>
     <mergeCell ref="A54:C54"/>
     <mergeCell ref="A55:C55"/>
     <mergeCell ref="J55:P55"/>
     <mergeCell ref="A56:C56"/>
     <mergeCell ref="J51:P54"/>
-    <mergeCell ref="C28:P28"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="C23:P23"/>
-    <mergeCell ref="C24:P24"/>
-    <mergeCell ref="C25:P25"/>
-    <mergeCell ref="C26:P26"/>
-    <mergeCell ref="C27:P27"/>
-    <mergeCell ref="C18:P18"/>
-    <mergeCell ref="C19:P19"/>
-    <mergeCell ref="C20:P20"/>
-    <mergeCell ref="C21:P21"/>
-    <mergeCell ref="C22:P22"/>
-    <mergeCell ref="C13:P13"/>
-    <mergeCell ref="C14:P14"/>
-    <mergeCell ref="C15:P15"/>
-    <mergeCell ref="C16:P16"/>
-    <mergeCell ref="C17:P17"/>
-    <mergeCell ref="A8:P8"/>
-    <mergeCell ref="C9:P9"/>
-    <mergeCell ref="C10:P10"/>
-    <mergeCell ref="C11:P11"/>
-    <mergeCell ref="C12:P12"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="I6:P6"/>
-    <mergeCell ref="A7:P7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.196850393700787" right="0.196850393700787" top="0.39370078740157499" bottom="0" header="0" footer="0"/>

</xml_diff>